<commit_message>
- Final Commit 10-01-2018
</commit_message>
<xml_diff>
--- a/assets/excels/NurseryExampleSheet.xlsx
+++ b/assets/excels/NurseryExampleSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajaj Patel.DESKTOP-N40AHF1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\greenworld\assets\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>Owner Name</t>
+  </si>
+  <si>
+    <t>Is Member ? (Yes/No)</t>
   </si>
 </sst>
 </file>
@@ -366,20 +372,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -394,6 +404,12 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>